<commit_message>
Move enumerator dashboard inputs to hfc_input.xlsx
</commit_message>
<xml_diff>
--- a/hfc_inputs.xlsx
+++ b/hfc_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="10" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="1. incomplete" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,14 @@
     <sheet name="10. dates" sheetId="10" r:id="rId10"/>
     <sheet name="11. outliers" sheetId="11" r:id="rId11"/>
     <sheet name="12. duration" sheetId="12" r:id="rId12"/>
+    <sheet name="enumdb" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="728">
   <si>
     <t>variable</t>
   </si>
@@ -1899,16 +1900,336 @@
   </si>
   <si>
     <t>over_ward_bound</t>
+  </si>
+  <si>
+    <t>dkrf_variables</t>
+  </si>
+  <si>
+    <t>missing_variables</t>
+  </si>
+  <si>
+    <t>duration_variables</t>
+  </si>
+  <si>
+    <t>submission_date</t>
+  </si>
+  <si>
+    <t>q3_1</t>
+  </si>
+  <si>
+    <t>q3_2_1</t>
+  </si>
+  <si>
+    <t>q3_6_phone</t>
+  </si>
+  <si>
+    <t>q3_8</t>
+  </si>
+  <si>
+    <t>q3_8_1_1</t>
+  </si>
+  <si>
+    <t>q3_8_2_1</t>
+  </si>
+  <si>
+    <t>q3_8_3</t>
+  </si>
+  <si>
+    <t>q3_10</t>
+  </si>
+  <si>
+    <t>q3_10_1_1</t>
+  </si>
+  <si>
+    <t>q3_10_2_1</t>
+  </si>
+  <si>
+    <t>q3_11</t>
+  </si>
+  <si>
+    <t>q3_13</t>
+  </si>
+  <si>
+    <t>q3_17</t>
+  </si>
+  <si>
+    <t>q3_19_1</t>
+  </si>
+  <si>
+    <t>q3_20</t>
+  </si>
+  <si>
+    <t>q3_24</t>
+  </si>
+  <si>
+    <t>q3_26_1</t>
+  </si>
+  <si>
+    <t>q4_2_2</t>
+  </si>
+  <si>
+    <t>q4_2_2_1</t>
+  </si>
+  <si>
+    <t>q4_2_2_2</t>
+  </si>
+  <si>
+    <t>q4_2_2_3</t>
+  </si>
+  <si>
+    <t>q4_2_2_4</t>
+  </si>
+  <si>
+    <t>q4_2_4</t>
+  </si>
+  <si>
+    <t>q4_2_5</t>
+  </si>
+  <si>
+    <t>q4_2_5_1_1</t>
+  </si>
+  <si>
+    <t>q4_2_5_1_2</t>
+  </si>
+  <si>
+    <t>q4_2_7</t>
+  </si>
+  <si>
+    <t>q4_2_8</t>
+  </si>
+  <si>
+    <t>q4_2_10</t>
+  </si>
+  <si>
+    <t>q4_2_11</t>
+  </si>
+  <si>
+    <t>q4_2_12_1</t>
+  </si>
+  <si>
+    <t>q4_2_14</t>
+  </si>
+  <si>
+    <t>q4_3</t>
+  </si>
+  <si>
+    <t>q4_3_1</t>
+  </si>
+  <si>
+    <t>q4_4_1</t>
+  </si>
+  <si>
+    <t>q4_4_2</t>
+  </si>
+  <si>
+    <t>q4_4_5</t>
+  </si>
+  <si>
+    <t>q4_4_5_1</t>
+  </si>
+  <si>
+    <t>q4_4_5_2</t>
+  </si>
+  <si>
+    <t>q4_4_5_3</t>
+  </si>
+  <si>
+    <t>q4_4_5_4</t>
+  </si>
+  <si>
+    <t>q4_4_7</t>
+  </si>
+  <si>
+    <t>q4_4_8</t>
+  </si>
+  <si>
+    <t>q4_4_11</t>
+  </si>
+  <si>
+    <t>q4_4_13</t>
+  </si>
+  <si>
+    <t>q4_4_14</t>
+  </si>
+  <si>
+    <t>q4_4_17</t>
+  </si>
+  <si>
+    <t>q4_5</t>
+  </si>
+  <si>
+    <t>q4_6_1</t>
+  </si>
+  <si>
+    <t>q4_6_4</t>
+  </si>
+  <si>
+    <t>q4_6_5</t>
+  </si>
+  <si>
+    <t>q4_6_7</t>
+  </si>
+  <si>
+    <t>q4_6_8</t>
+  </si>
+  <si>
+    <t>q4_6_9</t>
+  </si>
+  <si>
+    <t>q4_6_10</t>
+  </si>
+  <si>
+    <t>q4_6_11</t>
+  </si>
+  <si>
+    <t>q4_6_12</t>
+  </si>
+  <si>
+    <t>q4_8</t>
+  </si>
+  <si>
+    <t>q4_10_1</t>
+  </si>
+  <si>
+    <t>q4_10_2</t>
+  </si>
+  <si>
+    <t>q4_10_3</t>
+  </si>
+  <si>
+    <t>q4_10_4</t>
+  </si>
+  <si>
+    <t>q5_1</t>
+  </si>
+  <si>
+    <t>q5_3_1</t>
+  </si>
+  <si>
+    <t>q6_1</t>
+  </si>
+  <si>
+    <t>q6_3_1</t>
+  </si>
+  <si>
+    <t>q6_3_3</t>
+  </si>
+  <si>
+    <t>q6_3_4</t>
+  </si>
+  <si>
+    <t>q6_3_5</t>
+  </si>
+  <si>
+    <t>q6_4_4</t>
+  </si>
+  <si>
+    <t>q6_4_5</t>
+  </si>
+  <si>
+    <t>q6_5_5</t>
+  </si>
+  <si>
+    <t>q6_6</t>
+  </si>
+  <si>
+    <t>q6_6_1</t>
+  </si>
+  <si>
+    <t>q6_6_2_1</t>
+  </si>
+  <si>
+    <t>q7_2_1</t>
+  </si>
+  <si>
+    <t>q7_3_1</t>
+  </si>
+  <si>
+    <t>q7_3_1_1</t>
+  </si>
+  <si>
+    <t>q8_1_1</t>
+  </si>
+  <si>
+    <t>q8_3_1</t>
+  </si>
+  <si>
+    <t>q8_5_1</t>
+  </si>
+  <si>
+    <t>q8_5_2</t>
+  </si>
+  <si>
+    <t>q8_5_3</t>
+  </si>
+  <si>
+    <t>q8_6_1</t>
+  </si>
+  <si>
+    <t>q8_7_2</t>
+  </si>
+  <si>
+    <t>q9</t>
+  </si>
+  <si>
+    <t>q9_3</t>
+  </si>
+  <si>
+    <t>q3_1_1</t>
+  </si>
+  <si>
+    <t>c1_1_consent</t>
+  </si>
+  <si>
+    <t>c1_1_consent_sign</t>
+  </si>
+  <si>
+    <t>treatment</t>
+  </si>
+  <si>
+    <t>exclude_variables</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>text_audit</t>
+  </si>
+  <si>
+    <t>comfield1</t>
+  </si>
+  <si>
+    <t>comfield2</t>
+  </si>
+  <si>
+    <t>audio_audit</t>
+  </si>
+  <si>
+    <t>comfield3</t>
+  </si>
+  <si>
+    <t>comfield4</t>
+  </si>
+  <si>
+    <t>sdate</t>
+  </si>
+  <si>
+    <t>ta_*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1931,10 +2252,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2509,7 +2831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2606,6 +2928,560 @@
       </c>
       <c r="B1" t="s">
         <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E89"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>627</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>716</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>628</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>629</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>630</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>631</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>632</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>633</v>
+      </c>
+      <c r="D9" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>634</v>
+      </c>
+      <c r="D10" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>635</v>
+      </c>
+      <c r="D11" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>636</v>
+      </c>
+      <c r="D12" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>637</v>
+      </c>
+      <c r="D13" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>638</v>
+      </c>
+      <c r="D14" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>639</v>
+      </c>
+      <c r="D15" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>640</v>
+      </c>
+      <c r="D16" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>641</v>
+      </c>
+      <c r="D17" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>642</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>643</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>644</v>
+      </c>
+      <c r="D20" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>645</v>
+      </c>
+      <c r="D21" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="3" t="s">
+        <v>713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix formatting on enumerator dashboard
</commit_message>
<xml_diff>
--- a/hfc_inputs.xlsx
+++ b/hfc_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="6" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="1. incomplete" sheetId="1" r:id="rId1"/>
@@ -295,7 +295,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="27">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -5754,7 +5783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -5790,12 +5819,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5864,12 +5893,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$A1="startdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G1048576">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5927,12 +5956,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5946,7 +5975,7 @@
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -6209,13 +6238,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$A1="dkrf_variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$A1&lt;&gt;""</formula>
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>OR($A1&lt;&gt;"", $B1&lt;&gt;"", $C1&lt;&gt;"", $D1&lt;&gt;"", $E1&lt;&gt;"", $F1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6227,7 +6256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -6277,12 +6306,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6333,12 +6362,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="21" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6424,12 +6453,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6476,12 +6505,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6567,12 +6596,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E1048576">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7340,12 +7369,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7886,12 +7915,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G1048576">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7977,12 +8006,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>$A1="specify_variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add formatting for enumerator db and input and replacement sheets.
</commit_message>
<xml_diff>
--- a/hfc_inputs.xlsx
+++ b/hfc_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="1. incomplete" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="66">
   <si>
     <t>variable</t>
   </si>
@@ -54,12 +54,6 @@
     <t>hard_max</t>
   </si>
   <si>
-    <t>rent</t>
-  </si>
-  <si>
-    <t>size</t>
-  </si>
-  <si>
     <t>consent_value</t>
   </si>
   <si>
@@ -79,9 +73,6 @@
   </si>
   <si>
     <t>gpsLongitude</t>
-  </si>
-  <si>
-    <t>intstatus_check</t>
   </si>
   <si>
     <t>SubmissionDate</t>
@@ -171,9 +162,6 @@
     <t>assert</t>
   </si>
   <si>
-    <t>if</t>
-  </si>
-  <si>
     <t>dkrf_variable</t>
   </si>
   <si>
@@ -201,13 +189,7 @@
     <t>days</t>
   </si>
   <si>
-    <t>consentsigned</t>
-  </si>
-  <si>
     <t>enumid</t>
-  </si>
-  <si>
-    <t>stoptime</t>
   </si>
   <si>
     <t>gender</t>
@@ -219,34 +201,34 @@
     <t>pregnant</t>
   </si>
   <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>pregnant == .</t>
-  </si>
-  <si>
-    <t>sex == 0</t>
-  </si>
-  <si>
-    <t>salary == .</t>
-  </si>
-  <si>
-    <t>employmt == 0</t>
-  </si>
-  <si>
-    <t>occupation == .</t>
-  </si>
-  <si>
     <t xml:space="preserve">employyear </t>
-  </si>
-  <si>
-    <t>employyear == 4</t>
   </si>
   <si>
     <t>supid</t>
   </si>
   <si>
     <t>instatus</t>
+  </si>
+  <si>
+    <t>if_condition</t>
+  </si>
+  <si>
+    <t>pregnant==.</t>
+  </si>
+  <si>
+    <t>gender==0</t>
+  </si>
+  <si>
+    <t>salary==.</t>
+  </si>
+  <si>
+    <t>employmt==0</t>
+  </si>
+  <si>
+    <t>occupation==.</t>
+  </si>
+  <si>
+    <t>employyear==4</t>
   </si>
 </sst>
 </file>
@@ -284,47 +266,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <border>
         <left style="thin">
@@ -671,24 +627,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1102,6 +1040,677 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="47625"/>
+          <a:ext cx="3648075" cy="1828800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>HFC Check #</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng" baseline="0"/>
+            <a:t> 10</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" u="sng"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Check date</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> variables.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>This check verifies that:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>    1. survey start and end dates are unmissing</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>    2. survey start and end dates are equal</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>    3. survey start dates are not before start of data collection</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>    4. survey start dates are not after the current date</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>    5. survey start dates within the same geographic cluster </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>        are within X days of each other (OPTIONAL).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="1971675"/>
+          <a:ext cx="3667125" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>startdate</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the variable containing the survey start date. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="2686050"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>enddate</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>This column specifies the variable containing the survey end date. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="3381375"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>surveystart</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>This column specifies the variable containing date that data collection began.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="4076700"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>enum</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>area</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the variable representing geographic clusters.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="4772025"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>days</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the number of days to that surveys within the same cluster should fall within</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9715500" y="5476875"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>output_variable</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>id </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>enumerator</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t> are displayed.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9715500" y="6172200"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>notes</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -1494,7 +2103,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1866,23 +2475,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>id </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>and </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>enumerator</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t> are displayed.</a:t>
+            <a:t>This column specifies variables to exclude from the summary page.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -3088,6 +3681,345 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5572125" y="47625"/>
+          <a:ext cx="3648075" cy="1638300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>HFC Check # 5</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Check that follow up record</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>s match master</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>This check applies to follow up or post-census surveys. It checks relevant identification variables against a master tracking list to ensure the data are matching. The name of the master list is specified in the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>master_check.do </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>file. Note, that you must have </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>cfout</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t> installed for this check to work properly.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5572125" y="1790701"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>variable</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the names of the variables to check for matches in the master and follow up.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5581650" y="2476500"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>output_variable</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>id </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>enumerator</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t> are displayed.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5581650" y="3181350"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>notes</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -3160,7 +4092,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>This check verifies certain skip patterns and survey logic are obeyed. If the survey is properly programmed and tested using SurveyCTO, there should not be violations. However, we include these checks to help identify programming errors or to check for logic added after the survey start.</a:t>
+            <a:t>This check verifies certain skip patterns and survey logic are obeyed. If the survey is properly programmed and tested using SurveyCTO, there should be no violations. However, we include these checks to help identify programming errors or to check for logic added after the survey start.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3530,10 +4462,9 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>if</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>if_condition</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:r>
@@ -3549,7 +4480,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3873,7 +4804,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4521,7 +5452,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4793,677 +5724,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5572125" y="3571875"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>notes</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>933450</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8334375" y="47625"/>
-          <a:ext cx="3648075" cy="1828800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
-            <a:t>HFC Check #</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" u="sng" baseline="0"/>
-            <a:t> 10</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" u="sng"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>Check date</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t> variables.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>This check verifies that:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>    1. survey start and end dates are unmissing</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>    2. survey start and end dates are equal</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>    3. survey start dates are not before start of data collection</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>    4. survey start dates are not after the current date</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>    5. survey start dates within the same geographic cluster </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>        are within X days of each other (OPTIONAL).</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8334375" y="1971675"/>
-          <a:ext cx="3667125" cy="647700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="92D050"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>startdate</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies the variable containing the survey start date. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8334375" y="2686050"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="92D050"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>enddate</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>This column specifies the variable containing the survey end date. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="TextBox 6"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8334375" y="3381375"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="92D050"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>surveystart</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>This column specifies the variable containing date that data collection began.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="TextBox 7"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8334375" y="4076700"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>enum</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>area</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies the variable representing geographic clusters.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="TextBox 8"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8334375" y="4772025"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>days</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies the number of days to that surveys within the same cluster should fall within</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="TextBox 9"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9715500" y="5476875"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>id </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>and </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>enumerator</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t> are displayed.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="TextBox 10"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9715500" y="6172200"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5783,8 +6043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -5797,18 +6057,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -5819,12 +6079,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="25" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="24" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5851,19 +6111,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -5893,12 +6153,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$A1="startdate"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G1048576">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5911,8 +6171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -5922,29 +6182,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="6">
+        <v>3</v>
+      </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -5956,12 +6220,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5975,89 +6239,89 @@
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -6238,12 +6502,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F1">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$A1="dkrf_variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:F1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>OR($A1&lt;&gt;"", $B1&lt;&gt;"", $C1&lt;&gt;"", $D1&lt;&gt;"", $E1&lt;&gt;"", $F1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6264,7 +6528,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -6287,18 +6551,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6306,12 +6570,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="21" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6335,18 +6599,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -6354,7 +6618,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -6362,12 +6626,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6381,7 +6645,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -6391,74 +6655,74 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6469,52 +6733,47 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:3">
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:3">
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="17" priority="2">
+  <conditionalFormatting sqref="A1:C1">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="16" priority="1">
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6523,7 +6782,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -6533,75 +6792,75 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E1048576">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6625,175 +6884,175 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="3" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C32" s="3"/>
     </row>
@@ -7369,12 +7628,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7388,7 +7647,7 @@
   <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -7410,15 +7669,15 @@
         <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B2">
         <v>18</v>
@@ -7426,38 +7685,30 @@
       <c r="C2">
         <v>24</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
         <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7915,12 +8166,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:G1">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:G1048576">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7941,24 +8192,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3"/>
     </row>
@@ -8006,12 +8257,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C1">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$A1="specify_variable"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:C1048576">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update input file to reflect new options.
</commit_message>
<xml_diff>
--- a/hfc_inputs.xlsx
+++ b/hfc_inputs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="1. incomplete" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>variable</t>
   </si>
@@ -63,9 +63,6 @@
     <t>surveystart</t>
   </si>
   <si>
-    <t>iqr_multiplier</t>
-  </si>
-  <si>
     <t>submission_date</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>exclude_variable</t>
   </si>
   <si>
-    <t>output_variable</t>
-  </si>
-  <si>
     <t>coming soon</t>
   </si>
   <si>
@@ -106,6 +100,24 @@
   </si>
   <si>
     <t>if_condition</t>
+  </si>
+  <si>
+    <t>complete_percent</t>
+  </si>
+  <si>
+    <t>keep</t>
+  </si>
+  <si>
+    <t>keep_current</t>
+  </si>
+  <si>
+    <t>keep_master</t>
+  </si>
+  <si>
+    <t>multiplier</t>
+  </si>
+  <si>
+    <t>other_variable</t>
   </si>
 </sst>
 </file>
@@ -521,13 +533,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>942975</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -605,13 +617,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -680,13 +692,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -752,16 +764,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -770,7 +782,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6962775" y="2876550"/>
+          <a:off x="6972300" y="4000500"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -807,7 +819,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -840,16 +852,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -858,7 +870,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6962775" y="3571875"/>
+          <a:off x="6972300" y="4695825"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -912,13 +924,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1238250</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -930,7 +942,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9810750" y="314325"/>
+          <a:off x="11191875" y="314325"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -1079,6 +1091,78 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 13"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6962775" y="2914649"/>
+          <a:ext cx="3667125" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>complete_percent</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies a minimum non-missing percentage for each interview. Any interview that falls below this threshold will be flagged as incomplete and included in the output.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1647,7 +1731,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -1998,7 +2082,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>This check verifies whether certain continuous variables contain outliers, where an outlier is defined to be a certain multiple of the IQR.</a:t>
+            <a:t>This check verifies whether certain continuous variables contain outliers, where an outlier is defined to be a certain multiple of the IQR or SD (Note: IQR or SD is specified in the master_check file).</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2140,14 +2224,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>iqr_multiplier</a:t>
+            <a:t>multiplier</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies the multiple of the interquartile range that signifies an outlier.</a:t>
+            <a:t>This column specifies the multiple of the interquartile range or standard deviation that signifies an outlier.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -2212,7 +2296,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -3406,7 +3490,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -3971,7 +4055,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -4462,7 +4546,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -4741,13 +4825,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>933450</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -4840,13 +4924,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
@@ -4915,16 +4999,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4933,7 +5017,103 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5581650" y="2476500"/>
+          <a:off x="5581650" y="2476499"/>
+          <a:ext cx="3667125" cy="790576"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>keep_current</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies additional variable values from the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>data set in memory </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>to display in the output file. By default </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>id </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>enumerator</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t> are displayed.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5581650" y="4038600"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4970,30 +5150,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>notes</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>id </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>and </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>enumerator</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t> are displayed.</a:t>
+            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -5003,85 +5167,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5581650" y="3181350"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>notes</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>1238250</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -5093,7 +5185,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8429625" y="495300"/>
+          <a:off x="9810750" y="495300"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -5242,6 +5334,86 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5581650" y="3333749"/>
+          <a:ext cx="3667125" cy="609601"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>keep_master</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies additional variable values from the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>master tracking list </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>set to display in the output file. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5532,7 +5704,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -5882,13 +6054,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>942975</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -5966,13 +6138,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -6041,25 +6213,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4200525" y="2857500"/>
+          <a:off x="2819400" y="2867025"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6096,30 +6268,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>notes</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>id </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>and </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>enumerator</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t> are displayed.</a:t>
+            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -6129,85 +6285,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4200525" y="3562350"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>notes</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>1228725</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -6219,7 +6303,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8420100" y="600075"/>
+          <a:off x="7038975" y="600075"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -6913,7 +6997,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -7192,13 +7276,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>933450</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
@@ -7278,16 +7362,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7297,7 +7381,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5572125" y="2181225"/>
-          <a:ext cx="3667125" cy="600075"/>
+          <a:ext cx="3667125" cy="657225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7353,16 +7437,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7371,7 +7455,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5572125" y="2867025"/>
+          <a:off x="5572125" y="3810000"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7408,7 +7492,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>output_variable</a:t>
+            <a:t>keep</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
         </a:p>
@@ -7441,16 +7525,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7459,7 +7543,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5572125" y="3571875"/>
+          <a:off x="5572125" y="4514850"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7513,13 +7597,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>1238250</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -7531,7 +7615,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8429625" y="695325"/>
+          <a:off x="9810750" y="695325"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -7678,6 +7762,81 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5572125" y="2924175"/>
+          <a:ext cx="3667125" cy="790575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>other_variable</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the names of the original select_one or select_multiple questions containing the other choice options.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -7946,41 +8105,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" activeCellId="1" sqref="D20 A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:D1">
+  <conditionalFormatting sqref="A1:E1">
     <cfRule type="expression" dxfId="23" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:D1048576">
+  <conditionalFormatting sqref="A1:E1048576">
     <cfRule type="expression" dxfId="22" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
@@ -7994,7 +8156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
@@ -8011,16 +8173,16 @@
         <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -8062,7 +8224,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -8072,13 +8234,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="3"/>
     </row>
@@ -8119,7 +8281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E6"/>
     </sheetView>
   </sheetViews>
@@ -8127,22 +8289,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -8376,7 +8538,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -8389,7 +8551,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -8399,13 +8561,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -8435,7 +8597,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -8448,10 +8610,10 @@
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8478,7 +8640,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A2:B10"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -8488,10 +8650,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -8542,41 +8704,47 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="B3" s="3"/>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="5" spans="1:4">
       <c r="B5" s="3"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C5" s="3"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:C1">
+  <conditionalFormatting sqref="A1:D1">
     <cfRule type="expression" dxfId="15" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C1048576">
+  <conditionalFormatting sqref="A1:D1048576">
     <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
@@ -8591,7 +8759,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D6"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -8601,16 +8769,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -8654,635 +8822,552 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C602"/>
+  <dimension ref="A1:B602"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="C2" s="3"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="C4" s="3"/>
-    </row>
-    <row r="15" spans="1:3">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3">
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="C17" s="3"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="C19" s="3"/>
-    </row>
-    <row r="30" spans="1:3">
+    </row>
+    <row r="17" spans="1:2">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:3">
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="C32" s="3"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="C34" s="3"/>
-    </row>
-    <row r="45" spans="1:3">
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32" s="3"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-    </row>
-    <row r="46" spans="1:3">
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="C47" s="3"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="C49" s="3"/>
-    </row>
-    <row r="60" spans="1:3">
+    </row>
+    <row r="47" spans="1:2">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="B49" s="3"/>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-    </row>
-    <row r="61" spans="1:3">
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="C62" s="3"/>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="C64" s="3"/>
-    </row>
-    <row r="75" spans="1:3">
+    </row>
+    <row r="62" spans="1:2">
+      <c r="B62" s="3"/>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="B64" s="3"/>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-    </row>
-    <row r="76" spans="1:3">
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="C77" s="3"/>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="C79" s="3"/>
-    </row>
-    <row r="90" spans="1:3">
+    </row>
+    <row r="77" spans="1:2">
+      <c r="B77" s="3"/>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="B79" s="3"/>
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-    </row>
-    <row r="91" spans="1:3">
+    </row>
+    <row r="91" spans="1:2">
       <c r="A91" s="3"/>
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="C92" s="3"/>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="C94" s="3"/>
-    </row>
-    <row r="105" spans="1:3">
+    </row>
+    <row r="92" spans="1:2">
+      <c r="B92" s="3"/>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="B94" s="3"/>
+    </row>
+    <row r="105" spans="1:2">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
-    </row>
-    <row r="106" spans="1:3">
+    </row>
+    <row r="106" spans="1:2">
       <c r="A106" s="3"/>
-      <c r="B106" s="3"/>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="C107" s="3"/>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="C109" s="3"/>
-    </row>
-    <row r="120" spans="1:3">
+    </row>
+    <row r="107" spans="1:2">
+      <c r="B107" s="3"/>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="B109" s="3"/>
+    </row>
+    <row r="120" spans="1:2">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
-    </row>
-    <row r="121" spans="1:3">
+    </row>
+    <row r="121" spans="1:2">
       <c r="A121" s="3"/>
-      <c r="B121" s="3"/>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="C122" s="3"/>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="C124" s="3"/>
-    </row>
-    <row r="135" spans="1:3">
+    </row>
+    <row r="122" spans="1:2">
+      <c r="B122" s="3"/>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="B124" s="3"/>
+    </row>
+    <row r="135" spans="1:2">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
-      <c r="C135" s="3"/>
-    </row>
-    <row r="136" spans="1:3">
+    </row>
+    <row r="136" spans="1:2">
       <c r="A136" s="3"/>
-      <c r="B136" s="3"/>
-    </row>
-    <row r="137" spans="1:3">
-      <c r="C137" s="3"/>
-    </row>
-    <row r="139" spans="1:3">
-      <c r="C139" s="3"/>
-    </row>
-    <row r="150" spans="1:3">
+    </row>
+    <row r="137" spans="1:2">
+      <c r="B137" s="3"/>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="B139" s="3"/>
+    </row>
+    <row r="150" spans="1:2">
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
-      <c r="C150" s="3"/>
-    </row>
-    <row r="151" spans="1:3">
+    </row>
+    <row r="151" spans="1:2">
       <c r="A151" s="3"/>
-      <c r="B151" s="3"/>
-    </row>
-    <row r="152" spans="1:3">
-      <c r="C152" s="3"/>
-    </row>
-    <row r="154" spans="1:3">
-      <c r="C154" s="3"/>
-    </row>
-    <row r="165" spans="1:3">
+    </row>
+    <row r="152" spans="1:2">
+      <c r="B152" s="3"/>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="B154" s="3"/>
+    </row>
+    <row r="165" spans="1:2">
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
-      <c r="C165" s="3"/>
-    </row>
-    <row r="166" spans="1:3">
+    </row>
+    <row r="166" spans="1:2">
       <c r="A166" s="3"/>
-      <c r="B166" s="3"/>
-    </row>
-    <row r="167" spans="1:3">
-      <c r="C167" s="3"/>
-    </row>
-    <row r="169" spans="1:3">
-      <c r="C169" s="3"/>
-    </row>
-    <row r="180" spans="1:3">
+    </row>
+    <row r="167" spans="1:2">
+      <c r="B167" s="3"/>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="B169" s="3"/>
+    </row>
+    <row r="180" spans="1:2">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
-      <c r="C180" s="3"/>
-    </row>
-    <row r="181" spans="1:3">
+    </row>
+    <row r="181" spans="1:2">
       <c r="A181" s="3"/>
-      <c r="B181" s="3"/>
-    </row>
-    <row r="182" spans="1:3">
-      <c r="C182" s="3"/>
-    </row>
-    <row r="184" spans="1:3">
-      <c r="C184" s="3"/>
-    </row>
-    <row r="195" spans="1:3">
+    </row>
+    <row r="182" spans="1:2">
+      <c r="B182" s="3"/>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="B184" s="3"/>
+    </row>
+    <row r="195" spans="1:2">
       <c r="A195" s="3"/>
       <c r="B195" s="3"/>
-      <c r="C195" s="3"/>
-    </row>
-    <row r="196" spans="1:3">
+    </row>
+    <row r="196" spans="1:2">
       <c r="A196" s="3"/>
-      <c r="B196" s="3"/>
-    </row>
-    <row r="197" spans="1:3">
-      <c r="C197" s="3"/>
-    </row>
-    <row r="199" spans="1:3">
-      <c r="C199" s="3"/>
-    </row>
-    <row r="210" spans="1:3">
+    </row>
+    <row r="197" spans="1:2">
+      <c r="B197" s="3"/>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="B199" s="3"/>
+    </row>
+    <row r="210" spans="1:2">
       <c r="A210" s="3"/>
       <c r="B210" s="3"/>
-      <c r="C210" s="3"/>
-    </row>
-    <row r="211" spans="1:3">
+    </row>
+    <row r="211" spans="1:2">
       <c r="A211" s="3"/>
-      <c r="B211" s="3"/>
-    </row>
-    <row r="212" spans="1:3">
-      <c r="C212" s="3"/>
-    </row>
-    <row r="214" spans="1:3">
-      <c r="C214" s="3"/>
-    </row>
-    <row r="225" spans="1:3">
+    </row>
+    <row r="212" spans="1:2">
+      <c r="B212" s="3"/>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="B214" s="3"/>
+    </row>
+    <row r="225" spans="1:2">
       <c r="A225" s="3"/>
       <c r="B225" s="3"/>
-      <c r="C225" s="3"/>
-    </row>
-    <row r="226" spans="1:3">
+    </row>
+    <row r="226" spans="1:2">
       <c r="A226" s="3"/>
-      <c r="B226" s="3"/>
-    </row>
-    <row r="227" spans="1:3">
-      <c r="C227" s="3"/>
-    </row>
-    <row r="229" spans="1:3">
-      <c r="C229" s="3"/>
-    </row>
-    <row r="240" spans="1:3">
+    </row>
+    <row r="227" spans="1:2">
+      <c r="B227" s="3"/>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="B229" s="3"/>
+    </row>
+    <row r="240" spans="1:2">
       <c r="A240" s="3"/>
       <c r="B240" s="3"/>
-      <c r="C240" s="3"/>
-    </row>
-    <row r="241" spans="1:3">
+    </row>
+    <row r="241" spans="1:2">
       <c r="A241" s="3"/>
-      <c r="B241" s="3"/>
-    </row>
-    <row r="242" spans="1:3">
-      <c r="C242" s="3"/>
-    </row>
-    <row r="244" spans="1:3">
-      <c r="C244" s="3"/>
-    </row>
-    <row r="255" spans="1:3">
+    </row>
+    <row r="242" spans="1:2">
+      <c r="B242" s="3"/>
+    </row>
+    <row r="244" spans="1:2">
+      <c r="B244" s="3"/>
+    </row>
+    <row r="255" spans="1:2">
       <c r="A255" s="3"/>
       <c r="B255" s="3"/>
-      <c r="C255" s="3"/>
-    </row>
-    <row r="256" spans="1:3">
+    </row>
+    <row r="256" spans="1:2">
       <c r="A256" s="3"/>
-      <c r="B256" s="3"/>
-    </row>
-    <row r="257" spans="1:3">
-      <c r="C257" s="3"/>
-    </row>
-    <row r="259" spans="1:3">
-      <c r="C259" s="3"/>
-    </row>
-    <row r="270" spans="1:3">
+    </row>
+    <row r="257" spans="1:2">
+      <c r="B257" s="3"/>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="B259" s="3"/>
+    </row>
+    <row r="270" spans="1:2">
       <c r="A270" s="3"/>
       <c r="B270" s="3"/>
-      <c r="C270" s="3"/>
-    </row>
-    <row r="271" spans="1:3">
+    </row>
+    <row r="271" spans="1:2">
       <c r="A271" s="3"/>
-      <c r="B271" s="3"/>
-    </row>
-    <row r="272" spans="1:3">
-      <c r="C272" s="3"/>
-    </row>
-    <row r="274" spans="1:3">
-      <c r="C274" s="3"/>
-    </row>
-    <row r="285" spans="1:3">
+    </row>
+    <row r="272" spans="1:2">
+      <c r="B272" s="3"/>
+    </row>
+    <row r="274" spans="1:2">
+      <c r="B274" s="3"/>
+    </row>
+    <row r="285" spans="1:2">
       <c r="A285" s="3"/>
       <c r="B285" s="3"/>
-      <c r="C285" s="3"/>
-    </row>
-    <row r="286" spans="1:3">
+    </row>
+    <row r="286" spans="1:2">
       <c r="A286" s="3"/>
-      <c r="B286" s="3"/>
-    </row>
-    <row r="287" spans="1:3">
-      <c r="C287" s="3"/>
-    </row>
-    <row r="289" spans="1:3">
-      <c r="C289" s="3"/>
-    </row>
-    <row r="300" spans="1:3">
+    </row>
+    <row r="287" spans="1:2">
+      <c r="B287" s="3"/>
+    </row>
+    <row r="289" spans="1:2">
+      <c r="B289" s="3"/>
+    </row>
+    <row r="300" spans="1:2">
       <c r="A300" s="3"/>
       <c r="B300" s="3"/>
-      <c r="C300" s="3"/>
-    </row>
-    <row r="301" spans="1:3">
+    </row>
+    <row r="301" spans="1:2">
       <c r="A301" s="3"/>
-      <c r="B301" s="3"/>
-    </row>
-    <row r="302" spans="1:3">
-      <c r="C302" s="3"/>
-    </row>
-    <row r="304" spans="1:3">
-      <c r="C304" s="3"/>
-    </row>
-    <row r="315" spans="1:3">
+    </row>
+    <row r="302" spans="1:2">
+      <c r="B302" s="3"/>
+    </row>
+    <row r="304" spans="1:2">
+      <c r="B304" s="3"/>
+    </row>
+    <row r="315" spans="1:2">
       <c r="A315" s="3"/>
       <c r="B315" s="3"/>
-      <c r="C315" s="3"/>
-    </row>
-    <row r="316" spans="1:3">
+    </row>
+    <row r="316" spans="1:2">
       <c r="A316" s="3"/>
-      <c r="B316" s="3"/>
-    </row>
-    <row r="317" spans="1:3">
-      <c r="C317" s="3"/>
-    </row>
-    <row r="319" spans="1:3">
-      <c r="C319" s="3"/>
-    </row>
-    <row r="330" spans="1:3">
+    </row>
+    <row r="317" spans="1:2">
+      <c r="B317" s="3"/>
+    </row>
+    <row r="319" spans="1:2">
+      <c r="B319" s="3"/>
+    </row>
+    <row r="330" spans="1:2">
       <c r="A330" s="3"/>
       <c r="B330" s="3"/>
-      <c r="C330" s="3"/>
-    </row>
-    <row r="331" spans="1:3">
+    </row>
+    <row r="331" spans="1:2">
       <c r="A331" s="3"/>
-      <c r="B331" s="3"/>
-    </row>
-    <row r="332" spans="1:3">
-      <c r="C332" s="3"/>
-    </row>
-    <row r="334" spans="1:3">
-      <c r="C334" s="3"/>
-    </row>
-    <row r="345" spans="1:3">
+    </row>
+    <row r="332" spans="1:2">
+      <c r="B332" s="3"/>
+    </row>
+    <row r="334" spans="1:2">
+      <c r="B334" s="3"/>
+    </row>
+    <row r="345" spans="1:2">
       <c r="A345" s="3"/>
       <c r="B345" s="3"/>
-      <c r="C345" s="3"/>
-    </row>
-    <row r="346" spans="1:3">
+    </row>
+    <row r="346" spans="1:2">
       <c r="A346" s="3"/>
-      <c r="B346" s="3"/>
-    </row>
-    <row r="347" spans="1:3">
-      <c r="C347" s="3"/>
-    </row>
-    <row r="349" spans="1:3">
-      <c r="C349" s="3"/>
-    </row>
-    <row r="360" spans="1:3">
+    </row>
+    <row r="347" spans="1:2">
+      <c r="B347" s="3"/>
+    </row>
+    <row r="349" spans="1:2">
+      <c r="B349" s="3"/>
+    </row>
+    <row r="360" spans="1:2">
       <c r="A360" s="3"/>
       <c r="B360" s="3"/>
-      <c r="C360" s="3"/>
-    </row>
-    <row r="361" spans="1:3">
+    </row>
+    <row r="361" spans="1:2">
       <c r="A361" s="3"/>
-      <c r="B361" s="3"/>
-    </row>
-    <row r="362" spans="1:3">
-      <c r="C362" s="3"/>
-    </row>
-    <row r="364" spans="1:3">
-      <c r="C364" s="3"/>
-    </row>
-    <row r="375" spans="1:3">
+    </row>
+    <row r="362" spans="1:2">
+      <c r="B362" s="3"/>
+    </row>
+    <row r="364" spans="1:2">
+      <c r="B364" s="3"/>
+    </row>
+    <row r="375" spans="1:2">
       <c r="A375" s="3"/>
       <c r="B375" s="3"/>
-      <c r="C375" s="3"/>
-    </row>
-    <row r="376" spans="1:3">
+    </row>
+    <row r="376" spans="1:2">
       <c r="A376" s="3"/>
-      <c r="B376" s="3"/>
-    </row>
-    <row r="377" spans="1:3">
-      <c r="C377" s="3"/>
-    </row>
-    <row r="379" spans="1:3">
-      <c r="C379" s="3"/>
-    </row>
-    <row r="390" spans="1:3">
+    </row>
+    <row r="377" spans="1:2">
+      <c r="B377" s="3"/>
+    </row>
+    <row r="379" spans="1:2">
+      <c r="B379" s="3"/>
+    </row>
+    <row r="390" spans="1:2">
       <c r="A390" s="3"/>
       <c r="B390" s="3"/>
-      <c r="C390" s="3"/>
-    </row>
-    <row r="391" spans="1:3">
+    </row>
+    <row r="391" spans="1:2">
       <c r="A391" s="3"/>
-      <c r="B391" s="3"/>
-    </row>
-    <row r="392" spans="1:3">
-      <c r="C392" s="3"/>
-    </row>
-    <row r="394" spans="1:3">
-      <c r="C394" s="3"/>
-    </row>
-    <row r="405" spans="1:3">
+    </row>
+    <row r="392" spans="1:2">
+      <c r="B392" s="3"/>
+    </row>
+    <row r="394" spans="1:2">
+      <c r="B394" s="3"/>
+    </row>
+    <row r="405" spans="1:2">
       <c r="A405" s="3"/>
       <c r="B405" s="3"/>
-      <c r="C405" s="3"/>
-    </row>
-    <row r="406" spans="1:3">
+    </row>
+    <row r="406" spans="1:2">
       <c r="A406" s="3"/>
-      <c r="B406" s="3"/>
-    </row>
-    <row r="407" spans="1:3">
-      <c r="C407" s="3"/>
-    </row>
-    <row r="409" spans="1:3">
-      <c r="C409" s="3"/>
-    </row>
-    <row r="420" spans="1:3">
+    </row>
+    <row r="407" spans="1:2">
+      <c r="B407" s="3"/>
+    </row>
+    <row r="409" spans="1:2">
+      <c r="B409" s="3"/>
+    </row>
+    <row r="420" spans="1:2">
       <c r="A420" s="3"/>
       <c r="B420" s="3"/>
-      <c r="C420" s="3"/>
-    </row>
-    <row r="421" spans="1:3">
+    </row>
+    <row r="421" spans="1:2">
       <c r="A421" s="3"/>
-      <c r="B421" s="3"/>
-    </row>
-    <row r="422" spans="1:3">
-      <c r="C422" s="3"/>
-    </row>
-    <row r="424" spans="1:3">
-      <c r="C424" s="3"/>
-    </row>
-    <row r="435" spans="1:3">
+    </row>
+    <row r="422" spans="1:2">
+      <c r="B422" s="3"/>
+    </row>
+    <row r="424" spans="1:2">
+      <c r="B424" s="3"/>
+    </row>
+    <row r="435" spans="1:2">
       <c r="A435" s="3"/>
       <c r="B435" s="3"/>
-      <c r="C435" s="3"/>
-    </row>
-    <row r="436" spans="1:3">
+    </row>
+    <row r="436" spans="1:2">
       <c r="A436" s="3"/>
-      <c r="B436" s="3"/>
-    </row>
-    <row r="437" spans="1:3">
-      <c r="C437" s="3"/>
-    </row>
-    <row r="439" spans="1:3">
-      <c r="C439" s="3"/>
-    </row>
-    <row r="450" spans="1:3">
+    </row>
+    <row r="437" spans="1:2">
+      <c r="B437" s="3"/>
+    </row>
+    <row r="439" spans="1:2">
+      <c r="B439" s="3"/>
+    </row>
+    <row r="450" spans="1:2">
       <c r="A450" s="3"/>
       <c r="B450" s="3"/>
-      <c r="C450" s="3"/>
-    </row>
-    <row r="451" spans="1:3">
+    </row>
+    <row r="451" spans="1:2">
       <c r="A451" s="3"/>
-      <c r="B451" s="3"/>
-    </row>
-    <row r="452" spans="1:3">
-      <c r="C452" s="3"/>
-    </row>
-    <row r="454" spans="1:3">
-      <c r="C454" s="3"/>
-    </row>
-    <row r="465" spans="1:3">
+    </row>
+    <row r="452" spans="1:2">
+      <c r="B452" s="3"/>
+    </row>
+    <row r="454" spans="1:2">
+      <c r="B454" s="3"/>
+    </row>
+    <row r="465" spans="1:2">
       <c r="A465" s="3"/>
       <c r="B465" s="3"/>
-      <c r="C465" s="3"/>
-    </row>
-    <row r="466" spans="1:3">
+    </row>
+    <row r="466" spans="1:2">
       <c r="A466" s="3"/>
-      <c r="B466" s="3"/>
-    </row>
-    <row r="467" spans="1:3">
-      <c r="C467" s="3"/>
-    </row>
-    <row r="469" spans="1:3">
-      <c r="C469" s="3"/>
-    </row>
-    <row r="480" spans="1:3">
+    </row>
+    <row r="467" spans="1:2">
+      <c r="B467" s="3"/>
+    </row>
+    <row r="469" spans="1:2">
+      <c r="B469" s="3"/>
+    </row>
+    <row r="480" spans="1:2">
       <c r="A480" s="3"/>
       <c r="B480" s="3"/>
-      <c r="C480" s="3"/>
-    </row>
-    <row r="481" spans="1:3">
+    </row>
+    <row r="481" spans="1:2">
       <c r="A481" s="3"/>
-      <c r="B481" s="3"/>
-    </row>
-    <row r="482" spans="1:3">
-      <c r="C482" s="3"/>
-    </row>
-    <row r="484" spans="1:3">
-      <c r="C484" s="3"/>
-    </row>
-    <row r="495" spans="1:3">
+    </row>
+    <row r="482" spans="1:2">
+      <c r="B482" s="3"/>
+    </row>
+    <row r="484" spans="1:2">
+      <c r="B484" s="3"/>
+    </row>
+    <row r="495" spans="1:2">
       <c r="A495" s="3"/>
       <c r="B495" s="3"/>
-      <c r="C495" s="3"/>
-    </row>
-    <row r="496" spans="1:3">
+    </row>
+    <row r="496" spans="1:2">
       <c r="A496" s="3"/>
-      <c r="B496" s="3"/>
-    </row>
-    <row r="497" spans="1:3">
-      <c r="C497" s="3"/>
-    </row>
-    <row r="499" spans="1:3">
-      <c r="C499" s="3"/>
-    </row>
-    <row r="510" spans="1:3">
+    </row>
+    <row r="497" spans="1:2">
+      <c r="B497" s="3"/>
+    </row>
+    <row r="499" spans="1:2">
+      <c r="B499" s="3"/>
+    </row>
+    <row r="510" spans="1:2">
       <c r="A510" s="3"/>
       <c r="B510" s="3"/>
-      <c r="C510" s="3"/>
-    </row>
-    <row r="511" spans="1:3">
+    </row>
+    <row r="511" spans="1:2">
       <c r="A511" s="3"/>
-      <c r="B511" s="3"/>
-    </row>
-    <row r="512" spans="1:3">
-      <c r="C512" s="3"/>
-    </row>
-    <row r="514" spans="1:3">
-      <c r="C514" s="3"/>
-    </row>
-    <row r="525" spans="1:3">
+    </row>
+    <row r="512" spans="1:2">
+      <c r="B512" s="3"/>
+    </row>
+    <row r="514" spans="1:2">
+      <c r="B514" s="3"/>
+    </row>
+    <row r="525" spans="1:2">
       <c r="A525" s="3"/>
       <c r="B525" s="3"/>
-      <c r="C525" s="3"/>
-    </row>
-    <row r="526" spans="1:3">
+    </row>
+    <row r="526" spans="1:2">
       <c r="A526" s="3"/>
-      <c r="B526" s="3"/>
-    </row>
-    <row r="527" spans="1:3">
-      <c r="C527" s="3"/>
-    </row>
-    <row r="529" spans="1:3">
-      <c r="C529" s="3"/>
-    </row>
-    <row r="540" spans="1:3">
+    </row>
+    <row r="527" spans="1:2">
+      <c r="B527" s="3"/>
+    </row>
+    <row r="529" spans="1:2">
+      <c r="B529" s="3"/>
+    </row>
+    <row r="540" spans="1:2">
       <c r="A540" s="3"/>
       <c r="B540" s="3"/>
-      <c r="C540" s="3"/>
-    </row>
-    <row r="541" spans="1:3">
+    </row>
+    <row r="541" spans="1:2">
       <c r="A541" s="3"/>
-      <c r="B541" s="3"/>
-    </row>
-    <row r="542" spans="1:3">
-      <c r="C542" s="3"/>
-    </row>
-    <row r="544" spans="1:3">
-      <c r="C544" s="3"/>
-    </row>
-    <row r="555" spans="1:3">
+    </row>
+    <row r="542" spans="1:2">
+      <c r="B542" s="3"/>
+    </row>
+    <row r="544" spans="1:2">
+      <c r="B544" s="3"/>
+    </row>
+    <row r="555" spans="1:2">
       <c r="A555" s="3"/>
       <c r="B555" s="3"/>
-      <c r="C555" s="3"/>
-    </row>
-    <row r="556" spans="1:3">
+    </row>
+    <row r="556" spans="1:2">
       <c r="A556" s="3"/>
-      <c r="B556" s="3"/>
-    </row>
-    <row r="557" spans="1:3">
-      <c r="C557" s="3"/>
-    </row>
-    <row r="559" spans="1:3">
-      <c r="C559" s="3"/>
-    </row>
-    <row r="570" spans="1:3">
+    </row>
+    <row r="557" spans="1:2">
+      <c r="B557" s="3"/>
+    </row>
+    <row r="559" spans="1:2">
+      <c r="B559" s="3"/>
+    </row>
+    <row r="570" spans="1:2">
       <c r="A570" s="3"/>
       <c r="B570" s="3"/>
-      <c r="C570" s="3"/>
-    </row>
-    <row r="571" spans="1:3">
+    </row>
+    <row r="571" spans="1:2">
       <c r="A571" s="3"/>
-      <c r="B571" s="3"/>
-    </row>
-    <row r="572" spans="1:3">
-      <c r="C572" s="3"/>
-    </row>
-    <row r="574" spans="1:3">
-      <c r="C574" s="3"/>
-    </row>
-    <row r="585" spans="1:3">
+    </row>
+    <row r="572" spans="1:2">
+      <c r="B572" s="3"/>
+    </row>
+    <row r="574" spans="1:2">
+      <c r="B574" s="3"/>
+    </row>
+    <row r="585" spans="1:2">
       <c r="A585" s="3"/>
       <c r="B585" s="3"/>
-      <c r="C585" s="3"/>
-    </row>
-    <row r="586" spans="1:3">
+    </row>
+    <row r="586" spans="1:2">
       <c r="A586" s="3"/>
-      <c r="B586" s="3"/>
-    </row>
-    <row r="587" spans="1:3">
-      <c r="C587" s="3"/>
-    </row>
-    <row r="589" spans="1:3">
-      <c r="C589" s="3"/>
-    </row>
-    <row r="600" spans="1:3">
+    </row>
+    <row r="587" spans="1:2">
+      <c r="B587" s="3"/>
+    </row>
+    <row r="589" spans="1:2">
+      <c r="B589" s="3"/>
+    </row>
+    <row r="600" spans="1:2">
       <c r="A600" s="3"/>
       <c r="B600" s="3"/>
-      <c r="C600" s="3"/>
-    </row>
-    <row r="601" spans="1:3">
+    </row>
+    <row r="601" spans="1:2">
       <c r="A601" s="3"/>
-      <c r="B601" s="3"/>
-    </row>
-    <row r="602" spans="1:3">
-      <c r="C602" s="3"/>
+    </row>
+    <row r="602" spans="1:2">
+      <c r="B602" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:C1">
+  <conditionalFormatting sqref="A1:B1">
     <cfRule type="expression" dxfId="11" priority="3">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C1048576">
+  <conditionalFormatting sqref="A1:B1048576">
     <cfRule type="expression" dxfId="10" priority="2">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
@@ -9296,8 +9381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C4"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -9319,10 +9404,10 @@
         <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -9808,82 +9893,93 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="C5" s="3"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="B3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="D5" s="3"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="C9" s="3"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="C11" s="3"/>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="C15" s="3"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="C17" s="3"/>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:C1">
+  <conditionalFormatting sqref="A1:D1">
     <cfRule type="expression" dxfId="7" priority="2">
       <formula>$A1="specify_variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C1048576">
+  <conditionalFormatting sqref="A1:D1048576">
     <cfRule type="expression" dxfId="6" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>

</xml_diff>

<commit_message>
fix issue 62, modify excel templates for check #2
</commit_message>
<xml_diff>
--- a/hfc_inputs.xlsx
+++ b/hfc_inputs.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cboyer.IPA\Desktop\high-frequency-checks\exercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HFCCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1. incomplete" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
   <si>
     <t>variable</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>notes</t>
-  </si>
-  <si>
-    <t>other_unique</t>
   </si>
   <si>
     <t>assert</t>
@@ -123,7 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -3199,13 +3196,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>942975</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3280,16 +3277,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3298,8 +3295,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6962775" y="1600201"/>
-          <a:ext cx="3667125" cy="609600"/>
+          <a:off x="4200525" y="1600200"/>
+          <a:ext cx="3667125" cy="1419225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3345,7 +3342,19 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies the name of the variables that will be checked for duplicates (e.g. id, GPS, etc).</a:t>
+            <a:t>This column specifies the name of the variables that will be checked for duplicates (e.g. id, GPS, etc). </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Sometimes a combination of variables should be unique (e.g. multiple interviews with same respondent).  In that case, multiple variables can be input into one cell, separated by a space (e.g. id date).</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -3355,96 +3364,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="TextBox 8"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6962775" y="2276474"/>
-          <a:ext cx="3667125" cy="990601"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>other_unique</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>Sometimes a combination of variables should be unique (e.g. multiple interviews with same respondent). This column specifies a space separated list of additional variables, which in combination with </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>variable</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>, should be unique</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3453,7 +3382,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6962775" y="3343275"/>
+          <a:off x="4191000" y="3095625"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3523,16 +3452,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3541,7 +3470,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6962775" y="4029075"/>
+          <a:off x="4191000" y="3781425"/>
           <a:ext cx="3667125" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3595,13 +3524,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1238250</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -3613,7 +3542,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9810750" y="323850"/>
+          <a:off x="8429625" y="323850"/>
           <a:ext cx="1095375" cy="723900"/>
           <a:chOff x="10401300" y="1847850"/>
           <a:chExt cx="1095375" cy="723900"/>
@@ -5421,465 +5350,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6962775" y="47624"/>
-          <a:ext cx="3648075" cy="1495425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
-            <a:t>HFC Check # 6</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>Check skip</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t> patterns and survey logic.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
-            <a:t>This check verifies certain skip patterns and survey logic are obeyed. If the survey is properly programmed and tested using SurveyCTO, there should be no violations. However, we include these checks to help identify programming errors or to check for logic added after the survey start.</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6962775" y="1676400"/>
-          <a:ext cx="3667125" cy="600075"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="92D050"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>variable</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies the name of the survey status variable. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6962775" y="2343150"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="92D050"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>assert</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies a condition which should evaluate to true (e.g. sex == 1).</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6962775" y="3733800"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>keep</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>id </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>and </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>enumerator</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t> are displayed.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6962775" y="4429125"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFC000"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>notes</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="TextBox 6"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6962775" y="3038475"/>
-          <a:ext cx="3667125" cy="609600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="92D050"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>if_condition</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>This column specifies a condition under which the assertion should be true (e.g. pregnant == 1)</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -6045,6 +5515,478 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="TextBox 17"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6991350" y="66675"/>
+          <a:ext cx="3648075" cy="1828801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>HFC Check # 6</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Check skip</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> patterns and survey logic.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>This check verifies that skip patterns and survey logic are being obeyed. This check can test for logic added after the survey start. It can also flag soft checks that should be confirmed by enumerators, such as a household that reports paying school fees but has no children. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Patterns that are already enforced by the SurveyCTO form's programming do not need to be included. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="TextBox 18"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6991350" y="2009776"/>
+          <a:ext cx="3667125" cy="828675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>variable</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the names of the variables that are important for the logic test (e.g. children schoolfee). Multiple variables can be entered if separated by a space.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="TextBox 19"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6991350" y="2895601"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>assert</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies a condition which should evaluate to true (e.g. children &gt; 0).</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="TextBox 20"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6991350" y="4286251"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>keep</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies additional variable values to display in the output file. By default </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>id </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>enumerator</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t> are displayed.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="TextBox 21"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6991350" y="4981576"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>notes</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column is not used by Stata, rather it is included for the user's convenience to keep notes about inputs.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>990600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="TextBox 22"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6991350" y="3590926"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>if_condition</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies a condition under which the assertion should be true (e.g. schoolfee &gt; 0).</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -7918,6 +7860,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -7953,6 +7912,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8121,13 +8097,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>11</v>
@@ -8173,13 +8149,13 @@
         <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>11</v>
@@ -8234,10 +8210,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>11</v>
@@ -8289,16 +8265,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>10</v>
@@ -8538,7 +8514,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -8548,41 +8524,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:3">
       <c r="A3" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:D1">
+  <conditionalFormatting sqref="A1:C1">
     <cfRule type="expression" dxfId="21" priority="2">
       <formula>$A1="variable"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:D1048576">
+  <conditionalFormatting sqref="A1:C1048576">
     <cfRule type="expression" dxfId="20" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
@@ -8610,7 +8583,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>11</v>
@@ -8650,7 +8623,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
@@ -8706,7 +8679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -8717,10 +8690,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>11</v>
@@ -8759,7 +8732,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15"/>
@@ -8769,13 +8742,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>11</v>
@@ -9404,7 +9377,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>11</v>
@@ -9895,7 +9868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -9906,10 +9879,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>11</v>

</xml_diff>